<commit_message>
i modified all project
</commit_message>
<xml_diff>
--- a/hslim.xlsx
+++ b/hslim.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,13 +9,99 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+  <si>
+    <t>JSDSIDKDAD</t>
+  </si>
+  <si>
+    <t>GWWDWDWKDKWDKKDLDLJHSJCJ</t>
+  </si>
+  <si>
+    <t>SPSP[S]</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>DJWJDW[DW</t>
+  </si>
+  <si>
+    <t>WDJWJDND</t>
+  </si>
+  <si>
+    <t>DJKDM</t>
+  </si>
+  <si>
+    <t>WNNEF</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>MEF</t>
+  </si>
+  <si>
+    <t>JWWBBWE</t>
+  </si>
+  <si>
+    <t>WNBBF</t>
+  </si>
+  <si>
+    <t>WJ</t>
+  </si>
+  <si>
+    <t>EHDHEHEFJEE</t>
+  </si>
+  <si>
+    <t>DHGBD'</t>
+  </si>
+  <si>
+    <t>BVBND</t>
+  </si>
+  <si>
+    <t>DBVBD</t>
+  </si>
+  <si>
+    <t>DBVD</t>
+  </si>
+  <si>
+    <t>DBV D</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BD</t>
+  </si>
+  <si>
+    <t>FBVF</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DHHFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FJJF</t>
+  </si>
+  <si>
+    <t>F   F HHJF F</t>
+  </si>
+  <si>
+    <t>KKF</t>
+  </si>
+  <si>
+    <t>NNNF</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,13 +109,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -44,19 +149,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -98,7 +213,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +248,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +456,161 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F6" sqref="F3:H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>